<commit_message>
fix Price column and edit kach kach \ btn screen
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\Dataset\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F858CD21-12BC-406D-AC0C-D7D67133955A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7B25C5-6D61-47D6-9275-7CE8C53949F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5545B731-EC99-0F4C-9EAC-CB82643D319D}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2208" uniqueCount="630">
   <si>
     <t>Name</t>
   </si>
@@ -1948,9 +1948,6 @@
   </si>
   <si>
     <t>Wales</t>
-  </si>
-  <si>
-    <t>\</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2373,7 @@
   <dimension ref="A1:J551"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2961,8 +2958,8 @@
       <c r="E22">
         <v>36348</v>
       </c>
-      <c r="F22" t="s">
-        <v>630</v>
+      <c r="F22">
+        <v>20</v>
       </c>
       <c r="G22">
         <v>2014</v>

</xml_diff>